<commit_message>
test2 update by yangguang
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>第一次生成文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -29,6 +29,10 @@
   </si>
   <si>
     <t>update by yangguang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update by yangguang2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -378,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -414,6 +418,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>